<commit_message>
add Valuation calcs in Excel
</commit_message>
<xml_diff>
--- a/TixToGo/data/TixToGo.xlsx
+++ b/TixToGo/data/TixToGo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15760" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Exhibit 6" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,19 @@
     <sheet name="Exhibit 7c" sheetId="4" r:id="rId4"/>
     <sheet name="Exhibit 7d" sheetId="5" r:id="rId5"/>
     <sheet name="Exhibit 7e" sheetId="6" r:id="rId6"/>
+    <sheet name="Val" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="320">
   <si>
     <t>Number of Cities in Category</t>
   </si>
@@ -1016,20 +1022,84 @@
   <si>
     <t>ENDING CASH</t>
   </si>
+  <si>
+    <t>OpEx</t>
+  </si>
+  <si>
+    <t>EBIT</t>
+  </si>
+  <si>
+    <t>EBIAT</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Current Assets change</t>
+  </si>
+  <si>
+    <t>Current Liabilities change</t>
+  </si>
+  <si>
+    <t>Risk-Free Rate</t>
+  </si>
+  <si>
+    <t>Public Market Risk Premium</t>
+  </si>
+  <si>
+    <t>Stabilized Beta</t>
+  </si>
+  <si>
+    <t>Stabilized Discount Rate</t>
+  </si>
+  <si>
+    <t>Long-Term Growth Rate</t>
+  </si>
+  <si>
+    <t>FCF + TV</t>
+  </si>
+  <si>
+    <t>Free Cash Flows (FCF)</t>
+  </si>
+  <si>
+    <t>Terminal Value (TV)</t>
+  </si>
+  <si>
+    <t>Start-Up Period Beta</t>
+  </si>
+  <si>
+    <t>Angel Discount Rate</t>
+  </si>
+  <si>
+    <t>VC Discount Rate</t>
+  </si>
+  <si>
+    <t>Angel Valuation</t>
+  </si>
+  <si>
+    <t>VC Valuation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="10">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1052,16 +1122,69 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1069,12 +1192,191 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1110,12 +1412,164 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="95">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1416,24 +1870,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
-    <col min="3" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="12.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="15" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1460,12 +1914,12 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1940,7 @@
         <v>990000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1512,7 +1966,7 @@
         <v>2145000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1538,7 +1992,7 @@
         <v>821700</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1562,7 +2016,7 @@
         <v>508200</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1588,7 +2042,7 @@
         <v>1848000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +2068,7 @@
         <v>2805000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1640,7 +2094,7 @@
         <v>9157500</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1664,7 +2118,7 @@
         <v>1079100</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1688,7 +2142,7 @@
         <v>87450</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1714,7 +2168,7 @@
         <v>3613500</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1740,7 +2194,7 @@
         <v>577500</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1766,7 +2220,7 @@
         <v>29535000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1792,7 +2246,7 @@
         <v>136950</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1818,7 +2272,7 @@
         <v>704550</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1844,7 +2298,7 @@
         <v>2879250</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1866,7 +2320,7 @@
         <v>561000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1892,7 +2346,7 @@
         <v>610500</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1918,7 +2372,7 @@
         <v>759000</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1944,7 +2398,7 @@
         <v>620400</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1970,7 +2424,7 @@
         <v>580800</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1993,7 +2447,7 @@
         <v>60020400</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2018,6 +2472,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2025,23 +2484,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K107" sqref="J107:K107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" customWidth="1"/>
+    <col min="5" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="E3" t="s">
@@ -2051,13 +2510,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>35</v>
@@ -2065,7 +2524,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" t="s">
@@ -2078,7 +2537,7 @@
         <v>125966.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>39</v>
@@ -2090,7 +2549,7 @@
         <v>125966.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>40</v>
@@ -2098,7 +2557,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" t="s">
@@ -2107,7 +2566,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="D10" t="s">
@@ -2120,7 +2579,7 @@
         <v>115803.77</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="D11" t="s">
@@ -2133,7 +2592,7 @@
         <v>4968.1099999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -2147,7 +2606,7 @@
         <v>120771.88</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>45</v>
@@ -2159,7 +2618,7 @@
         <v>120771.88</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -2171,7 +2630,7 @@
         <v>5194.82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>47</v>
@@ -2179,7 +2638,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" t="s">
@@ -2188,7 +2647,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="D17" t="s">
@@ -2201,7 +2660,7 @@
         <v>1922.65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="D18" t="s">
@@ -2214,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="4" customFormat="1">
       <c r="C19" s="4" t="s">
         <v>51</v>
       </c>
@@ -2225,7 +2684,7 @@
         <v>1922.65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" t="s">
@@ -2234,7 +2693,7 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="D21" t="s">
@@ -2245,7 +2704,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="D22" t="s">
@@ -2256,7 +2715,7 @@
         <v>775.59</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="D23" t="s">
@@ -2267,7 +2726,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="D24" t="s">
@@ -2280,7 +2739,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="4" customFormat="1">
       <c r="C25" s="4" t="s">
         <v>117</v>
       </c>
@@ -2291,7 +2750,7 @@
         <v>4950.59</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" t="s">
@@ -2302,7 +2761,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" t="s">
@@ -2315,7 +2774,7 @@
         <v>548.07000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" t="s">
@@ -2324,7 +2783,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="D29" t="s">
@@ -2337,7 +2796,7 @@
         <v>40485.81</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="D30" t="s">
@@ -2348,7 +2807,7 @@
         <v>8270</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="D31" t="s">
@@ -2359,7 +2818,7 @@
         <v>1158.4100000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="4" customFormat="1">
       <c r="C32" s="4" t="s">
         <v>118</v>
       </c>
@@ -2370,7 +2829,7 @@
         <v>49914.22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" t="s">
@@ -2379,7 +2838,7 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="D34" t="s">
@@ -2392,7 +2851,7 @@
         <v>24171.62</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" t="s">
@@ -2403,7 +2862,7 @@
       </c>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="4" customFormat="1">
       <c r="C36" s="4" t="s">
         <v>119</v>
       </c>
@@ -2414,7 +2873,7 @@
         <v>24171.62</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" t="s">
@@ -2423,7 +2882,7 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="D38" t="s">
@@ -2436,7 +2895,7 @@
         <v>85472.27</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="D39" t="s">
@@ -2449,7 +2908,7 @@
         <v>14772.24</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="4" customFormat="1">
       <c r="C40" s="4" t="s">
         <v>120</v>
       </c>
@@ -2460,7 +2919,7 @@
         <v>100244.51</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" t="s">
@@ -2469,7 +2928,7 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="D42" t="s">
@@ -2482,7 +2941,7 @@
         <v>7761.47</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="D43" t="s">
@@ -2495,7 +2954,7 @@
         <v>81.55</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="4" customFormat="1">
       <c r="C44" s="4" t="s">
         <v>121</v>
       </c>
@@ -2506,7 +2965,7 @@
         <v>7843.02</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" t="s">
@@ -2515,7 +2974,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="D46" t="s">
@@ -2528,7 +2987,7 @@
         <v>5550</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="D47" t="s">
@@ -2541,7 +3000,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="D48" t="s">
@@ -2554,7 +3013,7 @@
         <v>4198.78</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="D49" t="s">
@@ -2567,7 +3026,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="D50" t="s">
@@ -2580,7 +3039,7 @@
         <v>705.23</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="4" customFormat="1">
       <c r="C51" s="4" t="s">
         <v>122</v>
       </c>
@@ -2591,7 +3050,7 @@
         <v>11902.01</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" t="s">
@@ -2600,7 +3059,7 @@
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="D53" t="s">
@@ -2613,7 +3072,7 @@
         <v>4536.67</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="D54" t="s">
@@ -2624,7 +3083,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="D55" t="s">
@@ -2635,7 +3094,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="D56" t="s">
@@ -2648,7 +3107,7 @@
         <v>531.20000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="D57" t="s">
@@ -2661,7 +3120,7 @@
         <v>142.04</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="D58" t="s">
@@ -2672,7 +3131,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="D59" t="s">
@@ -2685,7 +3144,7 @@
         <v>4034.79</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="4" customFormat="1">
       <c r="C60" s="4" t="s">
         <v>123</v>
       </c>
@@ -2696,7 +3155,7 @@
         <v>9244.7000000000007</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" t="s">
@@ -2709,7 +3168,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" t="s">
@@ -2718,7 +3177,7 @@
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="D63" t="s">
@@ -2729,7 +3188,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="D64" t="s">
@@ -2740,7 +3199,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="D65" t="s">
@@ -2753,7 +3212,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="4" customFormat="1">
       <c r="C66" s="4" t="s">
         <v>124</v>
       </c>
@@ -2764,7 +3223,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" t="s">
@@ -2773,7 +3232,7 @@
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="D68" t="s">
@@ -2784,7 +3243,7 @@
       </c>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="4" customFormat="1">
       <c r="C69" s="4" t="s">
         <v>125</v>
       </c>
@@ -2795,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" t="s">
@@ -2804,7 +3263,7 @@
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="D71" t="s">
@@ -2817,7 +3276,7 @@
         <v>698.18</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="D72" t="s">
@@ -2828,7 +3287,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="4" customFormat="1">
       <c r="C73" s="4" t="s">
         <v>126</v>
       </c>
@@ -2839,7 +3298,7 @@
         <v>698.18</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" t="s">
@@ -2848,7 +3307,7 @@
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="D75" t="s">
@@ -2861,7 +3320,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="4" customFormat="1">
       <c r="C76" s="4" t="s">
         <v>127</v>
       </c>
@@ -2872,7 +3331,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" t="s">
@@ -2885,7 +3344,7 @@
         <v>218.12</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" t="s">
@@ -2898,7 +3357,7 @@
         <v>183.5</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" t="s">
@@ -2911,7 +3370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" t="s">
@@ -2920,7 +3379,7 @@
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="D81" t="s">
@@ -2931,7 +3390,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="D82" t="s">
@@ -2944,7 +3403,7 @@
         <v>9968.75</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="D83" t="s">
@@ -2957,7 +3416,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="D84" t="s">
@@ -2970,7 +3429,7 @@
         <v>37883</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="D85" t="s">
@@ -2983,7 +3442,7 @@
         <v>537.27</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="C86" s="4" t="s">
         <v>128</v>
       </c>
@@ -2994,7 +3453,7 @@
         <v>51036.02</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" t="s">
@@ -3007,7 +3466,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" t="s">
@@ -3016,7 +3475,7 @@
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="D89" t="s">
@@ -3029,7 +3488,7 @@
         <v>1431.98</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="D90" t="s">
@@ -3042,7 +3501,7 @@
         <v>177.51</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="D91" t="s">
@@ -3055,7 +3514,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="C92" s="4" t="s">
         <v>129</v>
       </c>
@@ -3066,7 +3525,7 @@
         <v>3216.49</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" t="s">
@@ -3077,7 +3536,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" t="s">
@@ -3090,7 +3549,7 @@
         <v>1806.9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" t="s">
@@ -3103,7 +3562,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" t="s">
@@ -3114,7 +3573,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" s="4" customFormat="1">
       <c r="B97" s="4" t="s">
         <v>116</v>
       </c>
@@ -3125,7 +3584,7 @@
         <v>267374.90999999997</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" s="4" customFormat="1">
       <c r="B98" s="4" t="s">
         <v>130</v>
       </c>
@@ -3136,13 +3595,13 @@
         <v>-262180.09000000003</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" t="s">
@@ -3155,7 +3614,7 @@
         <v>12.86</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="C101" t="s">
         <v>133</v>
       </c>
@@ -3164,7 +3623,7 @@
       </c>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" s="4" customFormat="1">
       <c r="B102" s="4" t="s">
         <v>134</v>
       </c>
@@ -3175,28 +3634,28 @@
         <v>12.86</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" s="4" customFormat="1">
       <c r="B103" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="C104" t="s">
         <v>136</v>
       </c>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="C105" t="s">
         <v>137</v>
       </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="D106" t="s">
         <v>138</v>
       </c>
@@ -3207,7 +3666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="D107" t="s">
         <v>139</v>
       </c>
@@ -3216,7 +3675,7 @@
         <v>3888</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="D108" t="s">
         <v>140</v>
       </c>
@@ -3225,7 +3684,7 @@
         <v>178.32</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" s="4" customFormat="1">
       <c r="B109" s="4" t="s">
         <v>141</v>
       </c>
@@ -3236,7 +3695,7 @@
         <v>3610.32</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="C110" t="s">
         <v>142</v>
       </c>
@@ -3247,7 +3706,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" s="4" customFormat="1">
       <c r="B111" s="4" t="s">
         <v>143</v>
       </c>
@@ -3258,7 +3717,7 @@
         <v>4410.32</v>
       </c>
     </row>
-    <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" s="4" customFormat="1">
       <c r="B112" s="4" t="s">
         <v>144</v>
       </c>
@@ -3269,7 +3728,7 @@
         <v>-4397.46</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" s="4" customFormat="1">
       <c r="A113" s="4" t="s">
         <v>145</v>
       </c>
@@ -3282,6 +3741,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3289,24 +3753,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="1" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="G3" s="12">
         <v>36160</v>
       </c>
@@ -3314,14 +3778,14 @@
         <v>36280</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>147</v>
       </c>
       <c r="B4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>148</v>
@@ -3330,7 +3794,7 @@
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="D6" s="4" t="s">
@@ -3339,7 +3803,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="D7" s="4"/>
@@ -3353,7 +3817,7 @@
         <v>-11098.68</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="D8" s="4"/>
@@ -3365,7 +3829,7 @@
         <v>31558.31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="D9" s="4" t="s">
@@ -3378,7 +3842,7 @@
         <v>20459.63</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="D10" s="4" t="s">
@@ -3387,7 +3851,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="D11" s="4"/>
@@ -3401,7 +3865,7 @@
         <v>4964.51</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="D12" s="4" t="s">
@@ -3414,7 +3878,7 @@
         <v>4964.51</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="D13" s="4" t="s">
@@ -3423,7 +3887,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="D14" s="4"/>
@@ -3437,7 +3901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="D15" s="4"/>
@@ -3447,7 +3911,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="D16" s="4"/>
@@ -3459,7 +3923,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="D17" s="4"/>
@@ -3469,7 +3933,7 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="D18" s="4"/>
@@ -3483,7 +3947,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="D19" s="4"/>
@@ -3498,7 +3962,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="D20" s="4" t="s">
@@ -3511,7 +3975,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>164</v>
@@ -3524,7 +3988,7 @@
         <v>27143.14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>165</v>
@@ -3533,7 +3997,7 @@
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="D23" s="4"/>
@@ -3543,7 +4007,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="D24" s="4"/>
@@ -3557,7 +4021,7 @@
         <v>17358.669999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="D25" s="4"/>
@@ -3571,7 +4035,7 @@
         <v>-1292.94</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="D26" s="4"/>
@@ -3585,7 +4049,7 @@
         <v>4981.8</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="D27" s="4"/>
@@ -3599,7 +4063,7 @@
         <v>-284.64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="D28" s="4"/>
@@ -3613,7 +4077,7 @@
         <v>7046.75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="D29" s="4"/>
@@ -3627,7 +4091,7 @@
         <v>-835.89</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="D30" s="4"/>
@@ -3642,7 +4106,7 @@
         <v>26973.33</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>174</v>
@@ -3655,7 +4119,7 @@
         <v>26973.33</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>175</v>
@@ -3664,7 +4128,7 @@
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="D33" s="4"/>
@@ -3674,7 +4138,7 @@
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="D34" s="4"/>
@@ -3688,7 +4152,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="D35" s="4"/>
@@ -3702,7 +4166,7 @@
         <v>-255</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="D36" s="4"/>
@@ -3717,7 +4181,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="D37" s="4"/>
@@ -3731,7 +4195,7 @@
         <v>9716.85</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>181</v>
@@ -3744,14 +4208,14 @@
         <v>10361.85</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="D39" s="4"/>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="4" t="s">
         <v>182</v>
       </c>
@@ -3764,7 +4228,7 @@
         <v>64478.32</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
         <v>183</v>
       </c>
@@ -3773,7 +4237,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
         <v>184</v>
@@ -3782,7 +4246,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
@@ -3791,7 +4255,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3801,7 +4265,7 @@
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3816,7 +4280,7 @@
         <v>94912.85</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3831,7 +4295,7 @@
         <v>456.9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3842,7 +4306,7 @@
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3857,7 +4321,7 @@
         <v>144.68</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3872,7 +4336,7 @@
         <v>1212.93</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3885,7 +4349,7 @@
         <v>8676.57</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3898,7 +4362,7 @@
         <v>1681.09</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -3911,7 +4375,7 @@
         <v>373.83</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -3927,7 +4391,7 @@
         <v>12089.1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -3941,7 +4405,7 @@
         <v>107458.85</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3955,7 +4419,7 @@
         <v>144775.12</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -3965,7 +4429,7 @@
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3980,7 +4444,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3995,7 +4459,7 @@
         <v>2711.9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -4010,7 +4474,7 @@
         <v>634.24</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -4025,7 +4489,7 @@
         <v>537.66999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -4040,7 +4504,7 @@
         <v>63.53</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -4055,7 +4519,7 @@
         <v>85.61</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -4070,7 +4534,7 @@
         <v>8.31</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -4085,7 +4549,7 @@
         <v>76.150000000000006</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -4100,7 +4564,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -4113,7 +4577,7 @@
         <v>183.33</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -4127,7 +4591,7 @@
         <v>7745.74</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -4142,7 +4606,7 @@
         <v>49.01</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -4157,7 +4621,7 @@
         <v>203.25</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -4170,7 +4634,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="D72" s="16" t="s">
@@ -4179,7 +4643,7 @@
       <c r="G72" s="17"/>
       <c r="H72" s="17"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
@@ -4193,7 +4657,7 @@
         <v>310231.96999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="16" t="s">
@@ -4203,7 +4667,7 @@
       <c r="G74" s="17"/>
       <c r="H74" s="17"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -4213,7 +4677,7 @@
       <c r="G75" s="17"/>
       <c r="H75" s="17"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4228,7 +4692,7 @@
         <v>150595.1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -4243,7 +4707,7 @@
         <v>4529.3</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -4258,7 +4722,7 @@
         <v>9920.43</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -4273,7 +4737,7 @@
         <v>950.29</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -4287,7 +4751,7 @@
         <v>165995.12</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4" t="s">
@@ -4301,7 +4765,7 @@
         <v>165995.12</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
         <v>223</v>
@@ -4314,7 +4778,7 @@
         <v>476227.09</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
         <v>224</v>
@@ -4324,7 +4788,7 @@
       <c r="G83" s="17"/>
       <c r="H83" s="17"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -4339,7 +4803,7 @@
         <v>98996.26</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -4354,7 +4818,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -4369,7 +4833,7 @@
         <v>-246167.48</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -4384,7 +4848,7 @@
         <v>-266577.55</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
         <v>228</v>
@@ -4398,7 +4862,7 @@
         <v>-411748.77</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="4" t="s">
         <v>229</v>
       </c>
@@ -4412,7 +4876,7 @@
         <v>64478.32</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -4420,474 +4884,479 @@
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4896,25 +5365,25 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:G3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="C3" s="4" t="s">
         <v>249</v>
       </c>
@@ -4931,12 +5400,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>232</v>
@@ -4957,7 +5426,7 @@
         <v>156664954</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>233</v>
@@ -4978,7 +5447,7 @@
         <v>17280000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>234</v>
@@ -4999,7 +5468,7 @@
         <v>13440000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>235</v>
@@ -5020,7 +5489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -5040,14 +5509,14 @@
         <v>187384954</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="4"/>
       <c r="C10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>236</v>
       </c>
@@ -5067,7 +5536,7 @@
         <v>2447963</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1">
       <c r="A12" s="4" t="s">
         <v>237</v>
       </c>
@@ -5087,7 +5556,7 @@
         <v>184936991</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>238</v>
@@ -5108,15 +5577,15 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>240</v>
@@ -5137,7 +5606,7 @@
         <v>9514074</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>238</v>
@@ -5158,7 +5627,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>241</v>
@@ -5179,7 +5648,7 @@
         <v>97598730</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>238</v>
@@ -5200,7 +5669,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>242</v>
@@ -5221,7 +5690,7 @@
         <v>10076694</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>238</v>
@@ -5242,7 +5711,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1">
       <c r="A22" s="4" t="s">
         <v>243</v>
       </c>
@@ -5262,7 +5731,7 @@
         <v>117189498</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>238</v>
@@ -5283,12 +5752,30 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="4"/>
-      <c r="D24" s="18"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="21">
+        <f>C9-C11-C16-C18-C20</f>
+        <v>-950222</v>
+      </c>
+      <c r="D24" s="21">
+        <f t="shared" ref="D24:G24" si="0">D9-D11-D16-D18-D20</f>
+        <v>4233644</v>
+      </c>
+      <c r="E24" s="21">
+        <f t="shared" si="0"/>
+        <v>13940198</v>
+      </c>
+      <c r="F24" s="21">
+        <f t="shared" si="0"/>
+        <v>40451907</v>
+      </c>
+      <c r="G24" s="21">
+        <f t="shared" si="0"/>
+        <v>67747493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1">
       <c r="A25" s="4" t="s">
         <v>244</v>
       </c>
@@ -5308,7 +5795,7 @@
         <v>67747493</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
         <v>238</v>
@@ -5329,7 +5816,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
         <v>245</v>
@@ -5350,7 +5837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
         <v>246</v>
@@ -5371,7 +5858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="4" customFormat="1">
       <c r="A29" s="4" t="s">
         <v>247</v>
       </c>
@@ -5391,7 +5878,7 @@
         <v>677479493</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>248</v>
@@ -5412,7 +5899,7 @@
         <v>27098997</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="4" customFormat="1">
       <c r="A31" s="4" t="s">
         <v>145</v>
       </c>
@@ -5432,7 +5919,7 @@
         <v>40648496</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>238</v>
@@ -5455,6 +5942,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5466,19 +5959,19 @@
       <selection activeCell="B3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
+    <col min="2" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" s="4" t="s">
         <v>249</v>
       </c>
@@ -5495,7 +5988,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>255</v>
       </c>
@@ -5505,7 +5998,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>148</v>
       </c>
@@ -5515,7 +6008,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>256</v>
       </c>
@@ -5535,7 +6028,7 @@
         <v>91768480</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>257</v>
       </c>
@@ -5555,7 +6048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>258</v>
       </c>
@@ -5575,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -5595,14 +6088,14 @@
         <v>91768480</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>259</v>
       </c>
@@ -5622,7 +6115,7 @@
         <v>1228100</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>260</v>
       </c>
@@ -5642,7 +6135,7 @@
         <v>890258</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>261</v>
       </c>
@@ -5662,7 +6155,7 @@
         <v>337842</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>262</v>
       </c>
@@ -5682,14 +6175,14 @@
         <v>92106322</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>263</v>
       </c>
@@ -5699,7 +6192,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>264</v>
       </c>
@@ -5709,7 +6202,7 @@
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>265</v>
       </c>
@@ -5729,7 +6222,7 @@
         <v>5075726</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>266</v>
       </c>
@@ -5749,7 +6242,7 @@
         <v>704234</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>267</v>
       </c>
@@ -5769,7 +6262,7 @@
         <v>6774749</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>268</v>
       </c>
@@ -5789,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>269</v>
       </c>
@@ -5809,7 +6302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>270</v>
       </c>
@@ -5829,7 +6322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>271</v>
       </c>
@@ -5849,7 +6342,7 @@
         <v>12544709</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -5859,7 +6352,7 @@
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>272</v>
       </c>
@@ -5879,7 +6372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>273</v>
       </c>
@@ -5899,7 +6392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>222</v>
       </c>
@@ -5919,7 +6412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>274</v>
       </c>
@@ -5939,14 +6432,14 @@
         <v>12544709</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>224</v>
       </c>
@@ -5956,7 +6449,7 @@
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>275</v>
       </c>
@@ -5976,7 +6469,7 @@
         <v>4099000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>276</v>
       </c>
@@ -5996,7 +6489,7 @@
         <v>212000</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -6016,7 +6509,7 @@
         <v>75240613</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>228</v>
       </c>
@@ -6036,14 +6529,14 @@
         <v>79551613</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>278</v>
       </c>
@@ -6065,7 +6558,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6077,20 +6575,20 @@
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="C3" s="4" t="s">
         <v>249</v>
       </c>
@@ -6107,10 +6605,10 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>280</v>
       </c>
@@ -6131,7 +6629,7 @@
       </c>
       <c r="H5" s="21"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>281</v>
       </c>
@@ -6142,7 +6640,7 @@
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>145</v>
@@ -6164,7 +6662,7 @@
       </c>
       <c r="H7" s="21"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>282</v>
@@ -6186,7 +6684,7 @@
       </c>
       <c r="H8" s="21"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>283</v>
@@ -6208,7 +6706,7 @@
       </c>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>284</v>
@@ -6230,7 +6728,7 @@
       </c>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>285</v>
       </c>
@@ -6241,7 +6739,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>286</v>
@@ -6263,7 +6761,7 @@
       </c>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>266</v>
@@ -6285,7 +6783,7 @@
       </c>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>267</v>
@@ -6307,7 +6805,7 @@
       </c>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>287</v>
@@ -6329,7 +6827,7 @@
       </c>
       <c r="H15" s="21"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>288</v>
@@ -6351,7 +6849,7 @@
       </c>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>289</v>
@@ -6373,7 +6871,7 @@
       </c>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>290</v>
       </c>
@@ -6394,7 +6892,7 @@
       </c>
       <c r="H18" s="21"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="4"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -6403,7 +6901,7 @@
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>291</v>
       </c>
@@ -6414,7 +6912,7 @@
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>292</v>
       </c>
@@ -6425,7 +6923,7 @@
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>293</v>
@@ -6447,7 +6945,7 @@
       </c>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>258</v>
@@ -6469,7 +6967,7 @@
       </c>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>259</v>
@@ -6491,7 +6989,7 @@
       </c>
       <c r="H24" s="21"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>294</v>
@@ -6513,7 +7011,7 @@
       </c>
       <c r="H25" s="21"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
         <v>295</v>
@@ -6535,7 +7033,7 @@
       </c>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
         <v>296</v>
@@ -6557,7 +7055,7 @@
       </c>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>297</v>
       </c>
@@ -6578,7 +7076,7 @@
       </c>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="4"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
@@ -6587,7 +7085,7 @@
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>298</v>
       </c>
@@ -6608,7 +7106,7 @@
       </c>
       <c r="H30" s="21"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="4"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
@@ -6617,7 +7115,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>299</v>
       </c>
@@ -6638,13 +7136,673 @@
       </c>
       <c r="H32" s="21"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30" t="str">
+        <f>'Exhibit 7c'!C3</f>
+        <v>FY 1999</v>
+      </c>
+      <c r="E2" s="30" t="str">
+        <f>'Exhibit 7c'!D3</f>
+        <v>FY 2000</v>
+      </c>
+      <c r="F2" s="30" t="str">
+        <f>'Exhibit 7c'!E3</f>
+        <v>FY 2001</v>
+      </c>
+      <c r="G2" s="30" t="str">
+        <f>'Exhibit 7c'!F3</f>
+        <v>FY 2002</v>
+      </c>
+      <c r="H2" s="30" t="str">
+        <f>'Exhibit 7c'!G3</f>
+        <v>FY 2003</v>
+      </c>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="32"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0.08</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="35">
+        <v>2</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="C8" s="36">
+        <f>C4+C7*C5</f>
+        <v>0.19</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.27</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="C11" s="35">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="C12" s="36">
+        <f>C4+C11*C5</f>
+        <v>0.11</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="32"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="48">
+        <f>SUM('Exhibit 7c'!C5:C8)/10^6</f>
+        <v>2.9531999999999999E-2</v>
+      </c>
+      <c r="E16" s="48">
+        <f>SUM('Exhibit 7c'!D5:D8)/10^6</f>
+        <v>21.980360000000001</v>
+      </c>
+      <c r="F16" s="48">
+        <f>SUM('Exhibit 7c'!E5:E8)/10^6</f>
+        <v>57.321651000000003</v>
+      </c>
+      <c r="G16" s="48">
+        <f>SUM('Exhibit 7c'!F5:F8)/10^6</f>
+        <v>121.45330199999999</v>
+      </c>
+      <c r="H16" s="48">
+        <f>SUM('Exhibit 7c'!G5:G8)/10^6</f>
+        <v>187.38495399999999</v>
+      </c>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="48">
+        <f>('Exhibit 7c'!C11+'Exhibit 7c'!C16+'Exhibit 7c'!C18+'Exhibit 7c'!C20)/10^6</f>
+        <v>0.97975400000000001</v>
+      </c>
+      <c r="E17" s="48">
+        <f>('Exhibit 7c'!D11+'Exhibit 7c'!D16+'Exhibit 7c'!D18+'Exhibit 7c'!D20)/10^6</f>
+        <v>17.746715999999999</v>
+      </c>
+      <c r="F17" s="48">
+        <f>('Exhibit 7c'!E11+'Exhibit 7c'!E16+'Exhibit 7c'!E18+'Exhibit 7c'!E20)/10^6</f>
+        <v>43.381453</v>
+      </c>
+      <c r="G17" s="48">
+        <f>('Exhibit 7c'!F11+'Exhibit 7c'!F16+'Exhibit 7c'!F18+'Exhibit 7c'!F20)/10^6</f>
+        <v>81.001395000000002</v>
+      </c>
+      <c r="H17" s="48">
+        <f>('Exhibit 7c'!G11+'Exhibit 7c'!G16+'Exhibit 7c'!G18+'Exhibit 7c'!G20)/10^6</f>
+        <v>119.637461</v>
+      </c>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="48">
+        <f>D16-D17</f>
+        <v>-0.95022200000000001</v>
+      </c>
+      <c r="E18" s="48">
+        <f t="shared" ref="E18:H18" si="0">E16-E17</f>
+        <v>4.2336440000000017</v>
+      </c>
+      <c r="F18" s="48">
+        <f t="shared" si="0"/>
+        <v>13.940198000000002</v>
+      </c>
+      <c r="G18" s="48">
+        <f t="shared" si="0"/>
+        <v>40.451906999999991</v>
+      </c>
+      <c r="H18" s="48">
+        <f t="shared" si="0"/>
+        <v>67.747492999999992</v>
+      </c>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="C19" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="48">
+        <f>IF(D18&gt;0,(1-$C19)*D18,D18)</f>
+        <v>-0.95022200000000001</v>
+      </c>
+      <c r="E19" s="48">
+        <f t="shared" ref="E19:H19" si="1">IF(E18&gt;0,(1-$C19)*E18,E18)</f>
+        <v>2.540186400000001</v>
+      </c>
+      <c r="F19" s="48">
+        <f t="shared" si="1"/>
+        <v>8.3641188000000017</v>
+      </c>
+      <c r="G19" s="48">
+        <f t="shared" si="1"/>
+        <v>24.271144199999995</v>
+      </c>
+      <c r="H19" s="48">
+        <f t="shared" si="1"/>
+        <v>40.648495799999992</v>
+      </c>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="32"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="48">
+        <f>'Exhibit 7e'!C24/10^6</f>
+        <v>0.1226</v>
+      </c>
+      <c r="E21" s="48">
+        <f>'Exhibit 7e'!D24/10^6</f>
+        <v>0.3034</v>
+      </c>
+      <c r="F21" s="48">
+        <f>'Exhibit 7e'!E24/10^6</f>
+        <v>0.27460000000000001</v>
+      </c>
+      <c r="G21" s="48">
+        <f>'Exhibit 7e'!F24/10^6</f>
+        <v>0.25679999999999997</v>
+      </c>
+      <c r="H21" s="48">
+        <f>'Exhibit 7e'!G24/10^6</f>
+        <v>0.2707</v>
+      </c>
+      <c r="I21" s="41"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="48">
+        <f>'Exhibit 7e'!C8/10^6</f>
+        <v>1.4213999999999999E-2</v>
+      </c>
+      <c r="E22" s="48">
+        <f>'Exhibit 7e'!D8/10^6</f>
+        <v>9.6878000000000006E-2</v>
+      </c>
+      <c r="F22" s="48">
+        <f>'Exhibit 7e'!E8/10^6</f>
+        <v>0.23353299999999999</v>
+      </c>
+      <c r="G22" s="48">
+        <f>'Exhibit 7e'!F8/10^6</f>
+        <v>0.27826699999999999</v>
+      </c>
+      <c r="H22" s="48">
+        <f>'Exhibit 7e'!G8/10^6</f>
+        <v>0.26736700000000002</v>
+      </c>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="32"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="42"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="48">
+        <f>SUM('Exhibit 7d'!B7:B8)/10^6</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="48">
+        <f>(SUM('Exhibit 7d'!C7:C8)-SUM('Exhibit 7d'!B7:B8))/10^6</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="48">
+        <f>(SUM('Exhibit 7d'!D7:D8)-SUM('Exhibit 7d'!C7:C8))/10^6</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="48">
+        <f>(SUM('Exhibit 7d'!E7:E8)-SUM('Exhibit 7d'!D7:D8))/10^6</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="48">
+        <f>(SUM('Exhibit 7d'!F7:F8)-SUM('Exhibit 7d'!E7:E8))/10^6</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="41"/>
+      <c r="J24" s="42"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="48">
+        <f>SUM('Exhibit 7d'!B18:B23)/10^6</f>
+        <v>0.12992400000000001</v>
+      </c>
+      <c r="E25" s="48">
+        <f>(SUM('Exhibit 7d'!C18:C23)-SUM('Exhibit 7d'!B18:B23))/10^6</f>
+        <v>3.2158159999999998</v>
+      </c>
+      <c r="F25" s="48">
+        <f>(SUM('Exhibit 7d'!D18:D23)-SUM('Exhibit 7d'!C18:C23))/10^6</f>
+        <v>8.0243999999999996E-2</v>
+      </c>
+      <c r="G25" s="48">
+        <f>(SUM('Exhibit 7d'!E18:E23)-SUM('Exhibit 7d'!D18:D23))/10^6</f>
+        <v>4.5133150000000004</v>
+      </c>
+      <c r="H25" s="48">
+        <f>(SUM('Exhibit 7d'!F18:F23)-SUM('Exhibit 7d'!E18:E23))/10^6</f>
+        <v>4.6154099999999998</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="J25" s="42"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="32"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="42"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="48">
+        <f>D19-D21+D22-D24+D25</f>
+        <v>-0.92868399999999995</v>
+      </c>
+      <c r="E27" s="48">
+        <f t="shared" ref="E27:H27" si="2">E19-E21+E22-E24+E25</f>
+        <v>5.5494804000000002</v>
+      </c>
+      <c r="F27" s="48">
+        <f t="shared" si="2"/>
+        <v>8.4032958000000022</v>
+      </c>
+      <c r="G27" s="48">
+        <f t="shared" si="2"/>
+        <v>28.805926199999995</v>
+      </c>
+      <c r="H27" s="48">
+        <f t="shared" si="2"/>
+        <v>45.260572799999991</v>
+      </c>
+      <c r="I27" s="41"/>
+      <c r="J27" s="42"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="48">
+        <f>(1 +C13)*H27/(C12-C13)</f>
+        <v>672.44279588571408</v>
+      </c>
+      <c r="I28" s="44">
+        <f>H28/H16</f>
+        <v>3.5885634440303789</v>
+      </c>
+      <c r="J28" s="45">
+        <f>H28/H18</f>
+        <v>9.9257222091703703</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="C29" s="49">
+        <v>0</v>
+      </c>
+      <c r="D29" s="48">
+        <f>D27+D28</f>
+        <v>-0.92868399999999995</v>
+      </c>
+      <c r="E29" s="48">
+        <f t="shared" ref="E29:H29" si="3">E27+E28</f>
+        <v>5.5494804000000002</v>
+      </c>
+      <c r="F29" s="48">
+        <f t="shared" si="3"/>
+        <v>8.4032958000000022</v>
+      </c>
+      <c r="G29" s="48">
+        <f t="shared" si="3"/>
+        <v>28.805926199999995</v>
+      </c>
+      <c r="H29" s="48">
+        <f t="shared" si="3"/>
+        <v>717.70336868571405</v>
+      </c>
+      <c r="I29" s="41"/>
+      <c r="J29" s="42"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="32"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="42"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="C31" s="48">
+        <f>(1+$C8)*NPV($C8,C$29:$H$29)</f>
+        <v>323.24285013182089</v>
+      </c>
+      <c r="D31" s="48">
+        <f>(1+$C8)*NPV($C8,D$29:$H$29)</f>
+        <v>384.65899165686693</v>
+      </c>
+      <c r="E31" s="48">
+        <f>(1+$C8)*NPV($C8,E$29:$H$29)</f>
+        <v>458.84933403167162</v>
+      </c>
+      <c r="F31" s="48">
+        <f>(1+$C8)*NPV($C8,F$29:$H$29)</f>
+        <v>539.42682582168925</v>
+      </c>
+      <c r="G31" s="48">
+        <f>(1+$C8)*NPV($C8,G$29:$H$29)</f>
+        <v>631.9180007258102</v>
+      </c>
+      <c r="H31" s="48">
+        <f>(1+$C8)*NPV($C8,H$29:$H$29)</f>
+        <v>717.70336868571405</v>
+      </c>
+      <c r="I31" s="41"/>
+      <c r="J31" s="42"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="C32" s="48">
+        <f>(1+$C9)*NPV($C9,C$29:$H$29)</f>
+        <v>235.11817451962997</v>
+      </c>
+      <c r="D32" s="48">
+        <f>(1+$C9)*NPV($C9,D$29:$H$29)</f>
+        <v>298.60008163993007</v>
+      </c>
+      <c r="E32" s="48">
+        <f>(1+$C9)*NPV($C9,E$29:$H$29)</f>
+        <v>380.40153236271107</v>
+      </c>
+      <c r="F32" s="48">
+        <f>(1+$C9)*NPV($C9,F$29:$H$29)</f>
+        <v>476.06210599264307</v>
+      </c>
+      <c r="G32" s="48">
+        <f>(1+$C9)*NPV($C9,G$29:$H$29)</f>
+        <v>593.9266889446568</v>
+      </c>
+      <c r="H32" s="48">
+        <f>(1+$C9)*NPV($C9,H$29:$H$29)</f>
+        <v>717.70336868571405</v>
+      </c>
+      <c r="I32" s="41"/>
+      <c r="J32" s="42"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix errors in Excel source
</commit_message>
<xml_diff>
--- a/TixToGo/data/TixToGo.xlsx
+++ b/TixToGo/data/TixToGo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="325">
   <si>
     <t>Number of Cities in Category</t>
   </si>
@@ -1082,12 +1082,27 @@
   <si>
     <t>VC Valuation</t>
   </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Tax Loss</t>
+  </si>
+  <si>
+    <t>Taxable EBIT</t>
+  </si>
+  <si>
+    <t>FCF check tolerance</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -1097,9 +1112,10 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="0\x"/>
     <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1163,6 +1179,32 @@
       <sz val="12"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1184,7 +1226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1278,8 +1320,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1375,8 +1448,76 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1467,14 +1608,51 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="170" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="5" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="163">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1522,6 +1700,40 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1568,6 +1780,40 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
@@ -5364,8 +5610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5638,8 +5884,9 @@
       <c r="D18" s="21">
         <v>12480918</v>
       </c>
-      <c r="E18" s="21">
-        <v>31730291</v>
+      <c r="E18" s="51">
+        <f>31730291+21999</f>
+        <v>31752290</v>
       </c>
       <c r="F18" s="21">
         <v>64226275</v>
@@ -5754,26 +6001,6 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="4"/>
-      <c r="C24" s="21">
-        <f>C9-C11-C16-C18-C20</f>
-        <v>-950222</v>
-      </c>
-      <c r="D24" s="21">
-        <f t="shared" ref="D24:G24" si="0">D9-D11-D16-D18-D20</f>
-        <v>4233644</v>
-      </c>
-      <c r="E24" s="21">
-        <f t="shared" si="0"/>
-        <v>13940198</v>
-      </c>
-      <c r="F24" s="21">
-        <f t="shared" si="0"/>
-        <v>40451907</v>
-      </c>
-      <c r="G24" s="21">
-        <f t="shared" si="0"/>
-        <v>67747493</v>
-      </c>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1">
       <c r="A25" s="4" t="s">
@@ -6572,7 +6799,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6581,6 +6808,8 @@
     <col min="2" max="2" width="39.83203125" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6759,7 +6988,6 @@
       <c r="G12" s="21">
         <v>1708820</v>
       </c>
-      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4"/>
@@ -6781,7 +7009,6 @@
       <c r="G13" s="21">
         <v>177032</v>
       </c>
-      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4"/>
@@ -6800,10 +7027,10 @@
       <c r="F14" s="21">
         <v>2653371</v>
       </c>
-      <c r="G14" s="21">
-        <v>2279558</v>
-      </c>
-      <c r="H14" s="21"/>
+      <c r="G14" s="51">
+        <f>'Exhibit 7d'!F20-'Exhibit 7d'!E20</f>
+        <v>2729558</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="4"/>
@@ -6825,7 +7052,6 @@
       <c r="G15" s="21">
         <v>0</v>
       </c>
-      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="4"/>
@@ -7082,7 +7308,10 @@
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
+      <c r="G29" s="21">
+        <f>SUM(G7:G8,G12:G14)-SUM(G22:G27)</f>
+        <v>45260573</v>
+      </c>
       <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8">
@@ -7144,6 +7373,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7154,18 +7384,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J33"/>
+  <dimension ref="B2:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.1640625" style="25" customWidth="1"/>
     <col min="2" max="2" width="29.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="12.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="27" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="27" customWidth="1"/>
     <col min="9" max="10" width="5.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="25"/>
   </cols>
@@ -7352,19 +7586,23 @@
       <c r="J13" s="42"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="32"/>
-      <c r="C15" s="40"/>
+      <c r="B15" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="C15" s="50">
+        <v>1</v>
+      </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
@@ -7374,427 +7612,599 @@
       <c r="J15" s="42"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="48">
-        <f>SUM('Exhibit 7c'!C5:C8)/10^6</f>
-        <v>2.9531999999999999E-2</v>
-      </c>
-      <c r="E16" s="48">
-        <f>SUM('Exhibit 7c'!D5:D8)/10^6</f>
-        <v>21.980360000000001</v>
-      </c>
-      <c r="F16" s="48">
-        <f>SUM('Exhibit 7c'!E5:E8)/10^6</f>
-        <v>57.321651000000003</v>
-      </c>
-      <c r="G16" s="48">
-        <f>SUM('Exhibit 7c'!F5:F8)/10^6</f>
-        <v>121.45330199999999</v>
-      </c>
-      <c r="H16" s="48">
-        <f>SUM('Exhibit 7c'!G5:G8)/10^6</f>
-        <v>187.38495399999999</v>
-      </c>
-      <c r="I16" s="41"/>
-      <c r="J16" s="42"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="32" t="s">
-        <v>300</v>
-      </c>
+      <c r="B17" s="32"/>
       <c r="C17" s="40"/>
-      <c r="D17" s="48">
-        <f>('Exhibit 7c'!C11+'Exhibit 7c'!C16+'Exhibit 7c'!C18+'Exhibit 7c'!C20)/10^6</f>
-        <v>0.97975400000000001</v>
-      </c>
-      <c r="E17" s="48">
-        <f>('Exhibit 7c'!D11+'Exhibit 7c'!D16+'Exhibit 7c'!D18+'Exhibit 7c'!D20)/10^6</f>
-        <v>17.746715999999999</v>
-      </c>
-      <c r="F17" s="48">
-        <f>('Exhibit 7c'!E11+'Exhibit 7c'!E16+'Exhibit 7c'!E18+'Exhibit 7c'!E20)/10^6</f>
-        <v>43.381453</v>
-      </c>
-      <c r="G17" s="48">
-        <f>('Exhibit 7c'!F11+'Exhibit 7c'!F16+'Exhibit 7c'!F18+'Exhibit 7c'!F20)/10^6</f>
-        <v>81.001395000000002</v>
-      </c>
-      <c r="H17" s="48">
-        <f>('Exhibit 7c'!G11+'Exhibit 7c'!G16+'Exhibit 7c'!G18+'Exhibit 7c'!G20)/10^6</f>
-        <v>119.637461</v>
-      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="41"/>
       <c r="J17" s="42"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="32" t="s">
-        <v>301</v>
+        <v>231</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="48">
-        <f>D16-D17</f>
-        <v>-0.95022200000000001</v>
+        <f>SUM('Exhibit 7c'!C5:C8)/$C15</f>
+        <v>29532</v>
       </c>
       <c r="E18" s="48">
-        <f t="shared" ref="E18:H18" si="0">E16-E17</f>
-        <v>4.2336440000000017</v>
+        <f>SUM('Exhibit 7c'!D5:D8)/$C15</f>
+        <v>21980360</v>
       </c>
       <c r="F18" s="48">
-        <f t="shared" si="0"/>
-        <v>13.940198000000002</v>
+        <f>SUM('Exhibit 7c'!E5:E8)/$C15</f>
+        <v>57321651</v>
       </c>
       <c r="G18" s="48">
-        <f t="shared" si="0"/>
-        <v>40.451906999999991</v>
+        <f>SUM('Exhibit 7c'!F5:F8)/$C15</f>
+        <v>121453302</v>
       </c>
       <c r="H18" s="48">
-        <f t="shared" si="0"/>
-        <v>67.747492999999992</v>
+        <f>SUM('Exhibit 7c'!G5:G8)/$C15</f>
+        <v>187384954</v>
       </c>
       <c r="I18" s="41"/>
       <c r="J18" s="42"/>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="32" t="s">
-        <v>302</v>
-      </c>
-      <c r="C19" s="43">
-        <v>0.4</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C19" s="40"/>
       <c r="D19" s="48">
-        <f>IF(D18&gt;0,(1-$C19)*D18,D18)</f>
-        <v>-0.95022200000000001</v>
+        <f>('Exhibit 7c'!C11+'Exhibit 7c'!C16+'Exhibit 7c'!C18+'Exhibit 7c'!C20)/$C15</f>
+        <v>979754</v>
       </c>
       <c r="E19" s="48">
-        <f t="shared" ref="E19:H19" si="1">IF(E18&gt;0,(1-$C19)*E18,E18)</f>
-        <v>2.540186400000001</v>
+        <f>('Exhibit 7c'!D11+'Exhibit 7c'!D16+'Exhibit 7c'!D18+'Exhibit 7c'!D20)/$C15</f>
+        <v>17746716</v>
       </c>
       <c r="F19" s="48">
-        <f t="shared" si="1"/>
-        <v>8.3641188000000017</v>
+        <f>('Exhibit 7c'!E11+'Exhibit 7c'!E16+'Exhibit 7c'!E18+'Exhibit 7c'!E20)/$C15</f>
+        <v>43403452</v>
       </c>
       <c r="G19" s="48">
-        <f t="shared" si="1"/>
-        <v>24.271144199999995</v>
+        <f>('Exhibit 7c'!F11+'Exhibit 7c'!F16+'Exhibit 7c'!F18+'Exhibit 7c'!F20)/$C15</f>
+        <v>81001395</v>
       </c>
       <c r="H19" s="48">
-        <f t="shared" si="1"/>
-        <v>40.648495799999992</v>
+        <f>('Exhibit 7c'!G11+'Exhibit 7c'!G16+'Exhibit 7c'!G18+'Exhibit 7c'!G20)/$C15</f>
+        <v>119637461</v>
       </c>
       <c r="I19" s="41"/>
       <c r="J19" s="42"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="32"/>
+      <c r="B20" s="32" t="s">
+        <v>301</v>
+      </c>
       <c r="C20" s="40"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
+      <c r="D20" s="48">
+        <f>D18-D19</f>
+        <v>-950222</v>
+      </c>
+      <c r="E20" s="48">
+        <f t="shared" ref="E20:H20" si="0">E18-E19</f>
+        <v>4233644</v>
+      </c>
+      <c r="F20" s="48">
+        <f t="shared" si="0"/>
+        <v>13918199</v>
+      </c>
+      <c r="G20" s="48">
+        <f t="shared" si="0"/>
+        <v>40451907</v>
+      </c>
+      <c r="H20" s="48">
+        <f t="shared" si="0"/>
+        <v>67747493</v>
+      </c>
       <c r="I20" s="41"/>
       <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="32" t="s">
-        <v>303</v>
-      </c>
+      <c r="B21" s="32"/>
       <c r="C21" s="40"/>
-      <c r="D21" s="48">
-        <f>'Exhibit 7e'!C24/10^6</f>
-        <v>0.1226</v>
-      </c>
-      <c r="E21" s="48">
-        <f>'Exhibit 7e'!D24/10^6</f>
-        <v>0.3034</v>
-      </c>
-      <c r="F21" s="48">
-        <f>'Exhibit 7e'!E24/10^6</f>
-        <v>0.27460000000000001</v>
-      </c>
-      <c r="G21" s="48">
-        <f>'Exhibit 7e'!F24/10^6</f>
-        <v>0.25679999999999997</v>
-      </c>
-      <c r="H21" s="48">
-        <f>'Exhibit 7e'!G24/10^6</f>
-        <v>0.2707</v>
-      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
       <c r="I21" s="41"/>
       <c r="J21" s="42"/>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="32" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="C22" s="40"/>
       <c r="D22" s="48">
-        <f>'Exhibit 7e'!C8/10^6</f>
-        <v>1.4213999999999999E-2</v>
+        <f>MIN(C23,0)</f>
+        <v>0</v>
       </c>
       <c r="E22" s="48">
-        <f>'Exhibit 7e'!D8/10^6</f>
-        <v>9.6878000000000006E-2</v>
+        <f t="shared" ref="E22:H22" si="1">MIN(D23,0)</f>
+        <v>-950222</v>
       </c>
       <c r="F22" s="48">
-        <f>'Exhibit 7e'!E8/10^6</f>
-        <v>0.23353299999999999</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G22" s="48">
-        <f>'Exhibit 7e'!F8/10^6</f>
-        <v>0.27826699999999999</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H22" s="48">
-        <f>'Exhibit 7e'!G8/10^6</f>
-        <v>0.26736700000000002</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="42"/>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="32"/>
+      <c r="B23" s="32" t="s">
+        <v>322</v>
+      </c>
       <c r="C23" s="40"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
+      <c r="D23" s="48">
+        <f>D22+D20</f>
+        <v>-950222</v>
+      </c>
+      <c r="E23" s="48">
+        <f t="shared" ref="E23:H23" si="2">E22+E20</f>
+        <v>3283422</v>
+      </c>
+      <c r="F23" s="48">
+        <f t="shared" si="2"/>
+        <v>13918199</v>
+      </c>
+      <c r="G23" s="48">
+        <f t="shared" si="2"/>
+        <v>40451907</v>
+      </c>
+      <c r="H23" s="48">
+        <f t="shared" si="2"/>
+        <v>67747493</v>
+      </c>
       <c r="I23" s="41"/>
       <c r="J23" s="42"/>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="C24" s="40"/>
+        <v>302</v>
+      </c>
+      <c r="C24" s="43">
+        <v>0.4</v>
+      </c>
       <c r="D24" s="48">
-        <f>SUM('Exhibit 7d'!B7:B8)/10^6</f>
-        <v>0</v>
+        <f>D20-$C24*MAX(D23,0)</f>
+        <v>-950222</v>
       </c>
       <c r="E24" s="48">
-        <f>(SUM('Exhibit 7d'!C7:C8)-SUM('Exhibit 7d'!B7:B8))/10^6</f>
-        <v>0</v>
+        <f t="shared" ref="E24:H24" si="3">E20-$C24*MAX(E23,0)</f>
+        <v>2920275.2</v>
       </c>
       <c r="F24" s="48">
-        <f>(SUM('Exhibit 7d'!D7:D8)-SUM('Exhibit 7d'!C7:C8))/10^6</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8350919.3999999994</v>
       </c>
       <c r="G24" s="48">
-        <f>(SUM('Exhibit 7d'!E7:E8)-SUM('Exhibit 7d'!D7:D8))/10^6</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>24271144.199999999</v>
       </c>
       <c r="H24" s="48">
-        <f>(SUM('Exhibit 7d'!F7:F8)-SUM('Exhibit 7d'!E7:E8))/10^6</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>40648495.799999997</v>
       </c>
       <c r="I24" s="41"/>
       <c r="J24" s="42"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="32" t="s">
-        <v>306</v>
-      </c>
+      <c r="B25" s="32"/>
       <c r="C25" s="40"/>
-      <c r="D25" s="48">
-        <f>SUM('Exhibit 7d'!B18:B23)/10^6</f>
-        <v>0.12992400000000001</v>
-      </c>
-      <c r="E25" s="48">
-        <f>(SUM('Exhibit 7d'!C18:C23)-SUM('Exhibit 7d'!B18:B23))/10^6</f>
-        <v>3.2158159999999998</v>
-      </c>
-      <c r="F25" s="48">
-        <f>(SUM('Exhibit 7d'!D18:D23)-SUM('Exhibit 7d'!C18:C23))/10^6</f>
-        <v>8.0243999999999996E-2</v>
-      </c>
-      <c r="G25" s="48">
-        <f>(SUM('Exhibit 7d'!E18:E23)-SUM('Exhibit 7d'!D18:D23))/10^6</f>
-        <v>4.5133150000000004</v>
-      </c>
-      <c r="H25" s="48">
-        <f>(SUM('Exhibit 7d'!F18:F23)-SUM('Exhibit 7d'!E18:E23))/10^6</f>
-        <v>4.6154099999999998</v>
-      </c>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="41"/>
       <c r="J25" s="42"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="32"/>
+      <c r="B26" s="32" t="s">
+        <v>303</v>
+      </c>
       <c r="C26" s="40"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
+      <c r="D26" s="48">
+        <f>'Exhibit 7e'!C24/$C15</f>
+        <v>122600</v>
+      </c>
+      <c r="E26" s="48">
+        <f>'Exhibit 7e'!D24/$C15</f>
+        <v>303400</v>
+      </c>
+      <c r="F26" s="48">
+        <f>'Exhibit 7e'!E24/$C15</f>
+        <v>274600</v>
+      </c>
+      <c r="G26" s="48">
+        <f>'Exhibit 7e'!F24/$C15</f>
+        <v>256800</v>
+      </c>
+      <c r="H26" s="48">
+        <f>'Exhibit 7e'!G24/$C15</f>
+        <v>270700</v>
+      </c>
       <c r="I26" s="41"/>
       <c r="J26" s="42"/>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="32" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="48">
-        <f>D19-D21+D22-D24+D25</f>
-        <v>-0.92868399999999995</v>
+        <f>'Exhibit 7e'!C8/$C15</f>
+        <v>14214</v>
       </c>
       <c r="E27" s="48">
-        <f t="shared" ref="E27:H27" si="2">E19-E21+E22-E24+E25</f>
-        <v>5.5494804000000002</v>
+        <f>'Exhibit 7e'!D8/$C15</f>
+        <v>96878</v>
       </c>
       <c r="F27" s="48">
-        <f t="shared" si="2"/>
-        <v>8.4032958000000022</v>
+        <f>'Exhibit 7e'!E8/$C15</f>
+        <v>233533</v>
       </c>
       <c r="G27" s="48">
-        <f t="shared" si="2"/>
-        <v>28.805926199999995</v>
+        <f>'Exhibit 7e'!F8/$C15</f>
+        <v>278267</v>
       </c>
       <c r="H27" s="48">
-        <f t="shared" si="2"/>
-        <v>45.260572799999991</v>
+        <f>'Exhibit 7e'!G8/$C15</f>
+        <v>267367</v>
       </c>
       <c r="I27" s="41"/>
       <c r="J27" s="42"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="32" t="s">
-        <v>314</v>
-      </c>
+      <c r="B28" s="32"/>
       <c r="C28" s="40"/>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
-      <c r="H28" s="48">
-        <f>(1 +C13)*H27/(C12-C13)</f>
-        <v>672.44279588571408</v>
-      </c>
-      <c r="I28" s="44">
-        <f>H28/H16</f>
-        <v>3.5885634440303789</v>
-      </c>
-      <c r="J28" s="45">
-        <f>H28/H18</f>
-        <v>9.9257222091703703</v>
-      </c>
+      <c r="H28" s="34"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="C29" s="49">
-        <v>0</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="C29" s="40"/>
       <c r="D29" s="48">
-        <f>D27+D28</f>
-        <v>-0.92868399999999995</v>
+        <f>SUM('Exhibit 7d'!B7:B8)/$C15</f>
+        <v>0</v>
       </c>
       <c r="E29" s="48">
-        <f t="shared" ref="E29:H29" si="3">E27+E28</f>
-        <v>5.5494804000000002</v>
+        <f>(SUM('Exhibit 7d'!C7:C8)-SUM('Exhibit 7d'!B7:B8))/$C15</f>
+        <v>0</v>
       </c>
       <c r="F29" s="48">
-        <f t="shared" si="3"/>
-        <v>8.4032958000000022</v>
+        <f>(SUM('Exhibit 7d'!D7:D8)-SUM('Exhibit 7d'!C7:C8))/$C15</f>
+        <v>0</v>
       </c>
       <c r="G29" s="48">
-        <f t="shared" si="3"/>
-        <v>28.805926199999995</v>
+        <f>(SUM('Exhibit 7d'!E7:E8)-SUM('Exhibit 7d'!D7:D8))/$C15</f>
+        <v>0</v>
       </c>
       <c r="H29" s="48">
-        <f t="shared" si="3"/>
-        <v>717.70336868571405</v>
+        <f>(SUM('Exhibit 7d'!F7:F8)-SUM('Exhibit 7d'!E7:E8))/$C15</f>
+        <v>0</v>
       </c>
       <c r="I29" s="41"/>
       <c r="J29" s="42"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="32"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
+      <c r="B30" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="48">
+        <f>SUM('Exhibit 7d'!B18:B23)/$C15</f>
+        <v>129924</v>
+      </c>
+      <c r="E30" s="48">
+        <f>(SUM('Exhibit 7d'!C18:C23)-SUM('Exhibit 7d'!B18:B23))/$C15</f>
+        <v>3215816</v>
+      </c>
+      <c r="F30" s="48">
+        <f>(SUM('Exhibit 7d'!D18:D23)-SUM('Exhibit 7d'!C18:C23))/$C15</f>
+        <v>80244</v>
+      </c>
+      <c r="G30" s="48">
+        <f>(SUM('Exhibit 7d'!E18:E23)-SUM('Exhibit 7d'!D18:D23))/$C15</f>
+        <v>4513315</v>
+      </c>
+      <c r="H30" s="48">
+        <f>(SUM('Exhibit 7d'!F18:F23)-SUM('Exhibit 7d'!E18:E23))/$C15</f>
+        <v>4615410</v>
+      </c>
       <c r="I30" s="41"/>
       <c r="J30" s="42"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="32" t="s">
-        <v>318</v>
-      </c>
-      <c r="C31" s="48">
-        <f>(1+$C8)*NPV($C8,C$29:$H$29)</f>
-        <v>323.24285013182089</v>
-      </c>
-      <c r="D31" s="48">
-        <f>(1+$C8)*NPV($C8,D$29:$H$29)</f>
-        <v>384.65899165686693</v>
-      </c>
-      <c r="E31" s="48">
-        <f>(1+$C8)*NPV($C8,E$29:$H$29)</f>
-        <v>458.84933403167162</v>
-      </c>
-      <c r="F31" s="48">
-        <f>(1+$C8)*NPV($C8,F$29:$H$29)</f>
-        <v>539.42682582168925</v>
-      </c>
-      <c r="G31" s="48">
-        <f>(1+$C8)*NPV($C8,G$29:$H$29)</f>
-        <v>631.9180007258102</v>
-      </c>
-      <c r="H31" s="48">
-        <f>(1+$C8)*NPV($C8,H$29:$H$29)</f>
-        <v>717.70336868571405</v>
-      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
       <c r="I31" s="41"/>
       <c r="J31" s="42"/>
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="C32" s="48">
-        <f>(1+$C9)*NPV($C9,C$29:$H$29)</f>
-        <v>235.11817451962997</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="C32" s="40"/>
       <c r="D32" s="48">
-        <f>(1+$C9)*NPV($C9,D$29:$H$29)</f>
-        <v>298.60008163993007</v>
+        <f>D24-D26+D27-D29+D30</f>
+        <v>-928684</v>
       </c>
       <c r="E32" s="48">
-        <f>(1+$C9)*NPV($C9,E$29:$H$29)</f>
-        <v>380.40153236271107</v>
+        <f t="shared" ref="E32:H32" si="4">E24-E26+E27-E29+E30</f>
+        <v>5929569.2000000002</v>
       </c>
       <c r="F32" s="48">
-        <f>(1+$C9)*NPV($C9,F$29:$H$29)</f>
-        <v>476.06210599264307</v>
+        <f t="shared" si="4"/>
+        <v>8390096.3999999985</v>
       </c>
       <c r="G32" s="48">
-        <f>(1+$C9)*NPV($C9,G$29:$H$29)</f>
-        <v>593.9266889446568</v>
+        <f t="shared" si="4"/>
+        <v>28805926.199999999</v>
       </c>
       <c r="H32" s="48">
-        <f>(1+$C9)*NPV($C9,H$29:$H$29)</f>
-        <v>717.70336868571405</v>
+        <f t="shared" si="4"/>
+        <v>45260572.799999997</v>
       </c>
       <c r="I32" s="41"/>
       <c r="J32" s="42"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="47"/>
+      <c r="B33" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="C33" s="40"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="48">
+        <f>(1 +C13)*H32/(C12-C13)</f>
+        <v>672442795.88571417</v>
+      </c>
+      <c r="I33" s="44">
+        <f>H33/H18</f>
+        <v>3.5885634440303793</v>
+      </c>
+      <c r="J33" s="45">
+        <f>H33/H20</f>
+        <v>9.9257222091703703</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="C34" s="49">
+        <v>0</v>
+      </c>
+      <c r="D34" s="48">
+        <f>D32+D33</f>
+        <v>-928684</v>
+      </c>
+      <c r="E34" s="48">
+        <f t="shared" ref="E34:H34" si="5">E32+E33</f>
+        <v>5929569.2000000002</v>
+      </c>
+      <c r="F34" s="48">
+        <f t="shared" si="5"/>
+        <v>8390096.3999999985</v>
+      </c>
+      <c r="G34" s="48">
+        <f t="shared" si="5"/>
+        <v>28805926.199999999</v>
+      </c>
+      <c r="H34" s="48">
+        <f t="shared" si="5"/>
+        <v>717703368.68571413</v>
+      </c>
+      <c r="I34" s="41"/>
+      <c r="J34" s="42"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="32"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="42"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="C36" s="48">
+        <f>(1+$C8)*NPV($C8,C$34:$H$34)</f>
+        <v>323503422.73772931</v>
+      </c>
+      <c r="D36" s="48">
+        <f>(1+$C8)*NPV($C8,D$34:$H$34)</f>
+        <v>384969073.05789793</v>
+      </c>
+      <c r="E36" s="48">
+        <f>(1+$C8)*NPV($C8,E$34:$H$34)</f>
+        <v>459218330.89889848</v>
+      </c>
+      <c r="F36" s="48">
+        <f>(1+$C8)*NPV($C8,F$34:$H$34)</f>
+        <v>539413626.42168927</v>
+      </c>
+      <c r="G36" s="48">
+        <f>(1+$C8)*NPV($C8,G$34:$H$34)</f>
+        <v>631918000.72581029</v>
+      </c>
+      <c r="H36" s="48">
+        <f>(1+$C8)*NPV($C8,H$34:$H$34)</f>
+        <v>717703368.68571413</v>
+      </c>
+      <c r="I36" s="41"/>
+      <c r="J36" s="42"/>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="C37" s="48">
+        <f>(1+$C9)*NPV($C9,C$34:$H$34)</f>
+        <v>235347386.23247856</v>
+      </c>
+      <c r="D37" s="48">
+        <f>(1+$C9)*NPV($C9,D$34:$H$34)</f>
+        <v>298891180.51524782</v>
+      </c>
+      <c r="E37" s="48">
+        <f>(1+$C9)*NPV($C9,E$34:$H$34)</f>
+        <v>380771227.93436468</v>
+      </c>
+      <c r="F37" s="48">
+        <f>(1+$C9)*NPV($C9,F$34:$H$34)</f>
+        <v>476048906.59264314</v>
+      </c>
+      <c r="G37" s="48">
+        <f>(1+$C9)*NPV($C9,G$34:$H$34)</f>
+        <v>593926688.94465685</v>
+      </c>
+      <c r="H37" s="48">
+        <f>(1+$C9)*NPV($C9,H$34:$H$34)</f>
+        <v>717703368.68571413</v>
+      </c>
+      <c r="I37" s="41"/>
+      <c r="J37" s="42"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="47"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="52"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="56"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="C40" s="58">
+        <v>1.3</v>
+      </c>
+      <c r="D40" s="59">
+        <f>SUM('Exhibit 7e'!C7:C8,'Exhibit 7e'!C12:C17)-SUM('Exhibit 7e'!C22:C27)</f>
+        <v>-928684</v>
+      </c>
+      <c r="E40" s="59">
+        <f>SUM('Exhibit 7e'!D7:D8,'Exhibit 7e'!D12:D17)-SUM('Exhibit 7e'!D22:D27)</f>
+        <v>5929568</v>
+      </c>
+      <c r="F40" s="59">
+        <f>SUM('Exhibit 7e'!E7:E8,'Exhibit 7e'!E12:E17)-SUM('Exhibit 7e'!E22:E27)</f>
+        <v>8390096</v>
+      </c>
+      <c r="G40" s="59">
+        <f>SUM('Exhibit 7e'!F7:F8,'Exhibit 7e'!F12:F17)-SUM('Exhibit 7e'!F22:F27)</f>
+        <v>28805927</v>
+      </c>
+      <c r="H40" s="59">
+        <f>SUM('Exhibit 7e'!G7:G8,'Exhibit 7e'!G12:G17)-SUM('Exhibit 7e'!G22:G27)</f>
+        <v>45260573</v>
+      </c>
+      <c r="I40" s="60"/>
+      <c r="J40" s="61"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="C41" s="62" t="b">
+        <f>AND(D41:H41)</f>
+        <v>1</v>
+      </c>
+      <c r="D41" s="63" t="b">
+        <f>ABS(D32-D40)&lt;=$C40</f>
+        <v>1</v>
+      </c>
+      <c r="E41" s="63" t="b">
+        <f>ABS(E32-E40)&lt;=$C40</f>
+        <v>1</v>
+      </c>
+      <c r="F41" s="63" t="b">
+        <f>ABS(F32-F40)&lt;=$C40</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="63" t="b">
+        <f>ABS(G32-G40)&lt;=$C40</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="63" t="b">
+        <f>ABS(H32-H40)&lt;=$C40</f>
+        <v>1</v>
+      </c>
+      <c r="I41" s="60"/>
+      <c r="J41" s="61"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="64"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>